<commit_message>
updated capacity processing to create efficiencies table as part of the capacity list, also some minor updates to the index based on columns that were needed in the China project
</commit_message>
<xml_diff>
--- a/templates and indices/new plant list template and WEO DW index.xlsx
+++ b/templates and indices/new plant list template and WEO DW index.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HUNGERFORD_Z\localrepositories\plexos-model-setup\templates and indices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF0461B-E873-4C64-96E5-C587C92C97BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F688D4-5F31-44F9-9D91-4364E2022F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12660" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A2434ED0-D69B-4094-BCB0-7EE3461CB6A3}"/>
+    <workbookView xWindow="1620" yWindow="2205" windowWidth="23460" windowHeight="13530" activeTab="1" xr2:uid="{A2434ED0-D69B-4094-BCB0-7EE3461CB6A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4075,14 +4075,15 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I787"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
-      <selection activeCell="K133" sqref="K133"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K393" sqref="K393"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -4143,7 +4144,7 @@
         <v>1.24556E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>247</v>
       </c>
@@ -4172,7 +4173,7 @@
         <v>0.69955500000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>247</v>
       </c>
@@ -4201,7 +4202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>247</v>
       </c>
@@ -4230,7 +4231,7 @@
         <v>0.69955500000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>247</v>
       </c>
@@ -4259,7 +4260,7 @@
         <v>2.0615999999999999E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>247</v>
       </c>
@@ -4288,7 +4289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>247</v>
       </c>
@@ -4317,7 +4318,7 @@
         <v>0.261239</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>247</v>
       </c>
@@ -4346,7 +4347,7 @@
         <v>0.43810900000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>247</v>
       </c>
@@ -4375,7 +4376,7 @@
         <v>258.738</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>247</v>
       </c>
@@ -4404,7 +4405,7 @@
         <v>254.25200000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>247</v>
       </c>
@@ -4433,7 +4434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>247</v>
       </c>
@@ -4462,7 +4463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>247</v>
       </c>
@@ -4491,7 +4492,7 @@
         <v>254.25200000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>247</v>
       </c>
@@ -4520,7 +4521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>247</v>
       </c>
@@ -4549,7 +4550,7 @@
         <v>71.1006</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>247</v>
       </c>
@@ -4578,7 +4579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>247</v>
       </c>
@@ -4607,7 +4608,7 @@
         <v>0.97886399999999996</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>247</v>
       </c>
@@ -4636,7 +4637,7 @@
         <v>0.80900700000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>247</v>
       </c>
@@ -4665,7 +4666,7 @@
         <v>6.8423100000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>247</v>
       </c>
@@ -4694,7 +4695,7 @@
         <v>0.61143400000000003</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>247</v>
       </c>
@@ -4752,7 +4753,7 @@
         <v>1.7428699999999999E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>247</v>
       </c>
@@ -4781,7 +4782,7 @@
         <v>0.97886399999999996</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>247</v>
       </c>
@@ -4810,7 +4811,7 @@
         <v>0.97886399999999996</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>247</v>
       </c>
@@ -4839,7 +4840,7 @@
         <v>1.8510200000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>247</v>
       </c>
@@ -4868,7 +4869,7 @@
         <v>7.9925699999999997</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>247</v>
       </c>
@@ -4897,7 +4898,7 @@
         <v>2.9956299999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>247</v>
       </c>
@@ -4926,7 +4927,7 @@
         <v>4.9969400000000004</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>247</v>
       </c>
@@ -4955,7 +4956,7 @@
         <v>4.8355300000000003</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>247</v>
       </c>
@@ -4984,7 +4985,7 @@
         <v>1.1626200000000001E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>247</v>
       </c>
@@ -5013,7 +5014,7 @@
         <v>0.104425</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>247</v>
       </c>
@@ -5071,7 +5072,7 @@
         <v>0.229458</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>247</v>
       </c>
@@ -5100,7 +5101,7 @@
         <v>1288.72</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>247</v>
       </c>
@@ -5129,7 +5130,7 @@
         <v>393.27699999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>247</v>
       </c>
@@ -5187,7 +5188,7 @@
         <v>0.22958200000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>247</v>
       </c>
@@ -5245,7 +5246,7 @@
         <v>7.0023100000000005E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>247</v>
       </c>
@@ -5303,7 +5304,7 @@
         <v>0.15955900000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>247</v>
       </c>
@@ -5361,7 +5362,7 @@
         <v>3.0802700000000002E-5</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>247</v>
       </c>
@@ -5419,7 +5420,7 @@
         <v>4.35006E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>247</v>
       </c>
@@ -5477,7 +5478,7 @@
         <v>4.11493E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>247</v>
       </c>
@@ -5535,7 +5536,7 @@
         <v>7.4878299999999995E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>247</v>
       </c>
@@ -5564,7 +5565,7 @@
         <v>420.54599999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>247</v>
       </c>
@@ -5593,7 +5594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>247</v>
       </c>
@@ -5622,7 +5623,7 @@
         <v>0.172794</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>247</v>
       </c>
@@ -5651,7 +5652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>247</v>
       </c>
@@ -5680,7 +5681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>247</v>
       </c>
@@ -5709,7 +5710,7 @@
         <v>244.31700000000001</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>247</v>
       </c>
@@ -5738,7 +5739,7 @@
         <v>230.85</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>247</v>
       </c>
@@ -5796,7 +5797,7 @@
         <v>0.229458</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>247</v>
       </c>
@@ -5825,7 +5826,7 @@
         <v>1288.72</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>247</v>
       </c>
@@ -5854,7 +5855,7 @@
         <v>393.27699999999999</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>247</v>
       </c>
@@ -5912,7 +5913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>247</v>
       </c>
@@ -5941,7 +5942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>247</v>
       </c>
@@ -5970,7 +5971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>247</v>
       </c>
@@ -6028,7 +6029,7 @@
         <v>1.02586E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>247</v>
       </c>
@@ -6057,7 +6058,7 @@
         <v>5.76166</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>247</v>
       </c>
@@ -6086,7 +6087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>247</v>
       </c>
@@ -6144,7 +6145,7 @@
         <v>0.25305699999999998</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>247</v>
       </c>
@@ -6202,7 +6203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>247</v>
       </c>
@@ -6260,7 +6261,7 @@
         <v>8.8299099999999996E-5</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>247</v>
       </c>
@@ -6289,7 +6290,7 @@
         <v>0.495923</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>247</v>
       </c>
@@ -6318,7 +6319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>247</v>
       </c>
@@ -6376,7 +6377,7 @@
         <v>8.5217000000000001E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>247</v>
       </c>
@@ -6405,7 +6406,7 @@
         <v>478.613</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>247</v>
       </c>
@@ -6434,7 +6435,7 @@
         <v>468.88600000000002</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>247</v>
       </c>
@@ -6492,7 +6493,7 @@
         <v>1.32717E-4</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>247</v>
       </c>
@@ -6521,7 +6522,7 @@
         <v>0.74539200000000005</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>247</v>
       </c>
@@ -6550,7 +6551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>247</v>
       </c>
@@ -6608,7 +6609,7 @@
         <v>2.5727299999999997E-4</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>247</v>
       </c>
@@ -6637,7 +6638,7 @@
         <v>1.44495</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>247</v>
       </c>
@@ -6666,7 +6667,7 @@
         <v>0.714368</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>247</v>
       </c>
@@ -6695,7 +6696,7 @@
         <v>2.2347299999999999E-5</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>247</v>
       </c>
@@ -6724,7 +6725,7 @@
         <v>2.0072199999999998E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>247</v>
       </c>
@@ -6782,7 +6783,7 @@
         <v>0.74624599999999996</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>247</v>
       </c>
@@ -6840,7 +6841,7 @@
         <v>2.73035E-5</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>247</v>
       </c>
@@ -6869,7 +6870,7 @@
         <v>0.15334700000000001</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>247</v>
       </c>
@@ -6927,7 +6928,7 @@
         <v>1.7526499999999999E-3</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>247</v>
       </c>
@@ -6985,7 +6986,7 @@
         <v>1.4304900000000001E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>247</v>
       </c>
@@ -7014,7 +7015,7 @@
         <v>80.342200000000005</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>247</v>
       </c>
@@ -7043,7 +7044,7 @@
         <v>1.4204399999999999</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>247</v>
       </c>
@@ -7101,7 +7102,7 @@
         <v>2.2924799999999999E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>247</v>
       </c>
@@ -7130,7 +7131,7 @@
         <v>128.755</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>247</v>
       </c>
@@ -7159,7 +7160,7 @@
         <v>48.536999999999999</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>247</v>
       </c>
@@ -7188,7 +7189,7 @@
         <v>80.2179</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>247</v>
       </c>
@@ -7217,7 +7218,7 @@
         <v>77.633799999999994</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>247</v>
       </c>
@@ -7246,7 +7247,7 @@
         <v>1.8613900000000001E-3</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>247</v>
       </c>
@@ -7275,7 +7276,7 @@
         <v>1.6718900000000001</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>247</v>
       </c>
@@ -7333,7 +7334,7 @@
         <v>2.2924799999999999E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>247</v>
       </c>
@@ -7362,7 +7363,7 @@
         <v>128.755</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>247</v>
       </c>
@@ -7391,7 +7392,7 @@
         <v>48.536999999999999</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>247</v>
       </c>
@@ -7449,7 +7450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>247</v>
       </c>
@@ -7478,7 +7479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>247</v>
       </c>
@@ -7507,7 +7508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>247</v>
       </c>
@@ -7565,7 +7566,7 @@
         <v>0.64113500000000001</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>247</v>
       </c>
@@ -7623,7 +7624,7 @@
         <v>1.9637100000000001E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>247</v>
       </c>
@@ -7652,7 +7653,7 @@
         <v>110.29</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>247</v>
       </c>
@@ -7681,7 +7682,7 @@
         <v>2.34971</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>247</v>
       </c>
@@ -7739,7 +7740,7 @@
         <v>6.7425600000000003E-4</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>247</v>
       </c>
@@ -7768,7 +7769,7 @@
         <v>3.7868900000000001</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>247</v>
       </c>
@@ -7797,7 +7798,7 @@
         <v>1.4192400000000001</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>247</v>
       </c>
@@ -7826,7 +7827,7 @@
         <v>2.3676499999999998</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>247</v>
       </c>
@@ -7855,7 +7856,7 @@
         <v>2.3676499999999998</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>247</v>
       </c>
@@ -7913,7 +7914,7 @@
         <v>6.7425600000000003E-4</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>247</v>
       </c>
@@ -7971,7 +7972,7 @@
         <v>0.726352</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>247</v>
       </c>
@@ -8029,7 +8030,7 @@
         <v>0.45652100000000001</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>247</v>
       </c>
@@ -8087,7 +8088,7 @@
         <v>0.45549499999999998</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>247</v>
       </c>
@@ -8116,7 +8117,7 @@
         <v>2558.2399999999998</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>247</v>
       </c>
@@ -8145,7 +8146,7 @@
         <v>1307</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>247</v>
       </c>
@@ -8174,7 +8175,7 @@
         <v>1251.24</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>247</v>
       </c>
@@ -8203,7 +8204,7 @@
         <v>5875.13</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>247</v>
       </c>
@@ -8232,7 +8233,7 @@
         <v>450.78199999999998</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>247</v>
       </c>
@@ -8290,7 +8291,7 @@
         <v>2.4480600000000002E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>247</v>
       </c>
@@ -8348,7 +8349,7 @@
         <v>9.1753900000000003E-3</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>247</v>
       </c>
@@ -8406,7 +8407,7 @@
         <v>1.53052E-2</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>247</v>
       </c>
@@ -8464,7 +8465,7 @@
         <v>1.48109E-2</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>247</v>
       </c>
@@ -8522,7 +8523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>247</v>
       </c>
@@ -8580,7 +8581,7 @@
         <v>3.19847E-4</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>247</v>
       </c>
@@ -8638,7 +8639,7 @@
         <v>1.7415900000000001E-4</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>247</v>
       </c>
@@ -8696,7 +8697,7 @@
         <v>1.7428699999999999E-4</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>247</v>
       </c>
@@ -8754,7 +8755,7 @@
         <v>6.9725699999999995E-4</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>247</v>
       </c>
@@ -8783,7 +8784,7 @@
         <v>3.9160699999999999</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>247</v>
       </c>
@@ -8812,7 +8813,7 @@
         <v>0.51312000000000002</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>247</v>
       </c>
@@ -8870,7 +8871,7 @@
         <v>4.7963999999999997E-5</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>247</v>
       </c>
@@ -8899,7 +8900,7 @@
         <v>0.26938499999999999</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>247</v>
       </c>
@@ -8957,7 +8958,7 @@
         <v>0.16839299999999999</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>247</v>
       </c>
@@ -9015,7 +9016,7 @@
         <v>0.623888</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>247</v>
       </c>
@@ -9044,7 +9045,7 @@
         <v>3504</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>247</v>
       </c>
@@ -9073,7 +9074,7 @@
         <v>162.262</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>247</v>
       </c>
@@ -15424,7 +15425,7 @@
         <v>2026.06</v>
       </c>
     </row>
-    <row r="392" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>247</v>
       </c>
@@ -15453,7 +15454,7 @@
         <v>71.451700000000002</v>
       </c>
     </row>
-    <row r="393" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>247</v>
       </c>
@@ -15482,7 +15483,7 @@
         <v>8.1318907041177049</v>
       </c>
     </row>
-    <row r="394" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>247</v>
       </c>
@@ -15540,7 +15541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="396" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>247</v>
       </c>
@@ -15569,7 +15570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="397" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>247</v>
       </c>
@@ -15598,7 +15599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="398" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>247</v>
       </c>
@@ -15627,7 +15628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="399" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>247</v>
       </c>
@@ -15656,7 +15657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="400" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>247</v>
       </c>
@@ -15685,7 +15686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="401" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>247</v>
       </c>
@@ -15714,7 +15715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="402" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>247</v>
       </c>
@@ -15743,7 +15744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="403" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>247</v>
       </c>
@@ -15772,7 +15773,7 @@
         <v>245.13800000000001</v>
       </c>
     </row>
-    <row r="404" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>247</v>
       </c>
@@ -15801,7 +15802,7 @@
         <v>240.65199999999999</v>
       </c>
     </row>
-    <row r="405" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>247</v>
       </c>
@@ -15830,7 +15831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="406" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>247</v>
       </c>
@@ -15859,7 +15860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="407" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>247</v>
       </c>
@@ -15888,7 +15889,7 @@
         <v>240.65199999999999</v>
       </c>
     </row>
-    <row r="408" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>247</v>
       </c>
@@ -15917,7 +15918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="409" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>247</v>
       </c>
@@ -15946,7 +15947,7 @@
         <v>57.435699999999997</v>
       </c>
     </row>
-    <row r="410" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>247</v>
       </c>
@@ -15975,7 +15976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="411" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
         <v>247</v>
       </c>
@@ -16004,7 +16005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="412" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
         <v>247</v>
       </c>
@@ -16033,7 +16034,7 @@
         <v>0.412551</v>
       </c>
     </row>
-    <row r="413" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
         <v>247</v>
       </c>
@@ -16062,7 +16063,7 @@
         <v>5.8563599999999996</v>
       </c>
     </row>
-    <row r="414" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>247</v>
       </c>
@@ -16091,7 +16092,7 @@
         <v>0.77815400000000001</v>
       </c>
     </row>
-    <row r="415" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>247</v>
       </c>
@@ -16149,7 +16150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="417" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
         <v>247</v>
       </c>
@@ -16178,7 +16179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="418" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
         <v>247</v>
       </c>
@@ -16207,7 +16208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="419" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
         <v>247</v>
       </c>
@@ -16236,7 +16237,7 @@
         <v>1.6093200000000001</v>
       </c>
     </row>
-    <row r="420" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
         <v>247</v>
       </c>
@@ -16265,7 +16266,7 @@
         <v>3.15456</v>
       </c>
     </row>
-    <row r="421" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
         <v>247</v>
       </c>
@@ -16294,7 +16295,7 @@
         <v>1.6021700000000001</v>
       </c>
     </row>
-    <row r="422" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
         <v>247</v>
       </c>
@@ -16323,7 +16324,7 @@
         <v>1.5524</v>
       </c>
     </row>
-    <row r="423" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
         <v>247</v>
       </c>
@@ -16352,7 +16353,7 @@
         <v>1.4658100000000001</v>
       </c>
     </row>
-    <row r="424" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>247</v>
       </c>
@@ -16381,7 +16382,7 @@
         <v>3.6227099999999997E-5</v>
       </c>
     </row>
-    <row r="425" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
         <v>247</v>
       </c>
@@ -16410,7 +16411,7 @@
         <v>6.8848099999999995E-2</v>
       </c>
     </row>
-    <row r="426" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>247</v>
       </c>
@@ -16468,7 +16469,7 @@
         <v>0.238397</v>
       </c>
     </row>
-    <row r="428" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>247</v>
       </c>
@@ -16497,7 +16498,7 @@
         <v>1305.3800000000001</v>
       </c>
     </row>
-    <row r="429" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
         <v>247</v>
       </c>
@@ -16526,7 +16527,7 @@
         <v>397.541</v>
       </c>
     </row>
-    <row r="430" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
         <v>247</v>
       </c>
@@ -16584,7 +16585,7 @@
         <v>0.238397</v>
       </c>
     </row>
-    <row r="432" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
         <v>247</v>
       </c>
@@ -16642,7 +16643,7 @@
         <v>7.2601299999999994E-2</v>
       </c>
     </row>
-    <row r="434" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
         <v>247</v>
       </c>
@@ -16700,7 +16701,7 @@
         <v>0.165795</v>
       </c>
     </row>
-    <row r="436" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
         <v>247</v>
       </c>
@@ -16758,7 +16759,7 @@
         <v>3.1594299999999997E-5</v>
       </c>
     </row>
-    <row r="438" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
         <v>247</v>
       </c>
@@ -16816,7 +16817,7 @@
         <v>4.4378500000000001E-2</v>
       </c>
     </row>
-    <row r="440" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
         <v>247</v>
       </c>
@@ -16874,7 +16875,7 @@
         <v>4.08641E-2</v>
       </c>
     </row>
-    <row r="442" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
         <v>247</v>
       </c>
@@ -16932,7 +16933,7 @@
         <v>8.0338400000000004E-2</v>
       </c>
     </row>
-    <row r="444" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
         <v>247</v>
       </c>
@@ -16961,7 +16962,7 @@
         <v>439.90699999999998</v>
       </c>
     </row>
-    <row r="445" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
         <v>247</v>
       </c>
@@ -16990,7 +16991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="446" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
         <v>247</v>
       </c>
@@ -17019,7 +17020,7 @@
         <v>0.17299999999999999</v>
       </c>
     </row>
-    <row r="447" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
         <v>247</v>
       </c>
@@ -17048,7 +17049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="448" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
         <v>247</v>
       </c>
@@ -17077,7 +17078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="449" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
         <v>247</v>
       </c>
@@ -17106,7 +17107,7 @@
         <v>243.00200000000001</v>
       </c>
     </row>
-    <row r="450" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
         <v>247</v>
       </c>
@@ -17135,7 +17136,7 @@
         <v>223.75800000000001</v>
       </c>
     </row>
-    <row r="451" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
         <v>247</v>
       </c>
@@ -17193,7 +17194,7 @@
         <v>0.23821400000000001</v>
       </c>
     </row>
-    <row r="453" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
         <v>247</v>
       </c>
@@ -17222,7 +17223,7 @@
         <v>1304.3800000000001</v>
       </c>
     </row>
-    <row r="454" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
         <v>247</v>
       </c>
@@ -17251,7 +17252,7 @@
         <v>397.541</v>
       </c>
     </row>
-    <row r="455" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
         <v>247</v>
       </c>
@@ -17309,7 +17310,7 @@
         <v>1.82626E-4</v>
       </c>
     </row>
-    <row r="457" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
         <v>247</v>
       </c>
@@ -17338,7 +17339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="458" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
         <v>247</v>
       </c>
@@ -17367,7 +17368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="459" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
         <v>247</v>
       </c>
@@ -17425,7 +17426,7 @@
         <v>7.9828500000000003E-4</v>
       </c>
     </row>
-    <row r="461" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
         <v>247</v>
       </c>
@@ -17454,7 +17455,7 @@
         <v>4.3711500000000001</v>
       </c>
     </row>
-    <row r="462" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
         <v>247</v>
       </c>
@@ -17483,7 +17484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="463" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
         <v>247</v>
       </c>
@@ -17541,7 +17542,7 @@
         <v>0.27013500000000001</v>
       </c>
     </row>
-    <row r="465" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
         <v>247</v>
       </c>
@@ -17599,7 +17600,7 @@
         <v>1.82626E-4</v>
       </c>
     </row>
-    <row r="467" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
         <v>247</v>
       </c>
@@ -17657,7 +17658,7 @@
         <v>4.7024200000000003E-5</v>
       </c>
     </row>
-    <row r="469" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
         <v>247</v>
       </c>
@@ -17686,7 +17687,7 @@
         <v>0.25748900000000002</v>
       </c>
     </row>
-    <row r="470" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
         <v>247</v>
       </c>
@@ -17715,7 +17716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="471" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
         <v>247</v>
       </c>
@@ -17773,7 +17774,7 @@
         <v>8.5915199999999997E-2</v>
       </c>
     </row>
-    <row r="473" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A473" t="s">
         <v>247</v>
       </c>
@@ -17802,7 +17803,7 @@
         <v>470.44400000000002</v>
       </c>
     </row>
-    <row r="474" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
         <v>247</v>
       </c>
@@ -17831,7 +17832,7 @@
         <v>460.89800000000002</v>
       </c>
     </row>
-    <row r="475" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A475" t="s">
         <v>247</v>
       </c>
@@ -17889,7 +17890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="477" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
         <v>247</v>
       </c>
@@ -17918,7 +17919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="478" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A478" t="s">
         <v>247</v>
       </c>
@@ -17947,7 +17948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="479" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A479" t="s">
         <v>247</v>
       </c>
@@ -18005,7 +18006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="481" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
         <v>247</v>
       </c>
@@ -18034,7 +18035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="482" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
         <v>247</v>
       </c>
@@ -18063,7 +18064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="483" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A483" t="s">
         <v>247</v>
       </c>
@@ -18092,7 +18093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="484" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
         <v>247</v>
       </c>
@@ -18121,7 +18122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="485" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A485" t="s">
         <v>247</v>
       </c>
@@ -18179,7 +18180,7 @@
         <v>0.72913499999999998</v>
       </c>
     </row>
-    <row r="487" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
         <v>247</v>
       </c>
@@ -18237,7 +18238,7 @@
         <v>2.51291E-5</v>
       </c>
     </row>
-    <row r="489" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
         <v>247</v>
       </c>
@@ -18266,7 +18267,7 @@
         <v>0.137599</v>
       </c>
     </row>
-    <row r="490" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
         <v>247</v>
       </c>
@@ -18324,7 +18325,7 @@
         <v>8.7000800000000002E-4</v>
       </c>
     </row>
-    <row r="492" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
         <v>247</v>
       </c>
@@ -18382,7 +18383,7 @@
         <v>1.1776200000000001E-2</v>
       </c>
     </row>
-    <row r="494" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
         <v>247</v>
       </c>
@@ -18411,7 +18412,7 @@
         <v>64.482699999999994</v>
       </c>
     </row>
-    <row r="495" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A495" t="s">
         <v>247</v>
       </c>
@@ -18440,7 +18441,7 @@
         <v>1.1907099999999999</v>
       </c>
     </row>
-    <row r="496" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A496" t="s">
         <v>247</v>
       </c>
@@ -18498,7 +18499,7 @@
         <v>3.1229099999999999E-2</v>
       </c>
     </row>
-    <row r="498" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A498" t="s">
         <v>247</v>
       </c>
@@ -18527,7 +18528,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="499" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A499" t="s">
         <v>247</v>
       </c>
@@ -18556,7 +18557,7 @@
         <v>86.849100000000007</v>
       </c>
     </row>
-    <row r="500" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A500" t="s">
         <v>247</v>
       </c>
@@ -18585,7 +18586,7 @@
         <v>84.151200000000003</v>
       </c>
     </row>
-    <row r="501" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A501" t="s">
         <v>247</v>
       </c>
@@ -18614,7 +18615,7 @@
         <v>79.457499999999996</v>
       </c>
     </row>
-    <row r="502" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A502" t="s">
         <v>247</v>
       </c>
@@ -18643,7 +18644,7 @@
         <v>1.9637700000000001E-3</v>
       </c>
     </row>
-    <row r="503" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A503" t="s">
         <v>247</v>
       </c>
@@ -18672,7 +18673,7 @@
         <v>3.7320700000000002</v>
       </c>
     </row>
-    <row r="504" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="504" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A504" t="s">
         <v>247</v>
       </c>
@@ -18730,7 +18731,7 @@
         <v>3.1229099999999999E-2</v>
       </c>
     </row>
-    <row r="506" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A506" t="s">
         <v>247</v>
       </c>
@@ -18759,7 +18760,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="507" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="507" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A507" t="s">
         <v>247</v>
       </c>
@@ -18788,7 +18789,7 @@
         <v>86.849100000000007</v>
       </c>
     </row>
-    <row r="508" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A508" t="s">
         <v>247</v>
       </c>
@@ -18846,7 +18847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="510" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A510" t="s">
         <v>247</v>
       </c>
@@ -18875,7 +18876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="511" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A511" t="s">
         <v>247</v>
       </c>
@@ -18904,7 +18905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="512" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A512" t="s">
         <v>247</v>
       </c>
@@ -18962,7 +18963,7 @@
         <v>0.62404000000000004</v>
       </c>
     </row>
-    <row r="514" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="514" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A514" t="s">
         <v>247</v>
       </c>
@@ -19020,7 +19021,7 @@
         <v>1.8997199999999999E-2</v>
       </c>
     </row>
-    <row r="516" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="516" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A516" t="s">
         <v>247</v>
       </c>
@@ -19049,7 +19050,7 @@
         <v>104.02200000000001</v>
       </c>
     </row>
-    <row r="517" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="517" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A517" t="s">
         <v>247</v>
       </c>
@@ -19078,7 +19079,7 @@
         <v>3.54623</v>
       </c>
     </row>
-    <row r="518" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="518" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A518" t="s">
         <v>247</v>
       </c>
@@ -19136,7 +19137,7 @@
         <v>6.9180999999999995E-4</v>
       </c>
     </row>
-    <row r="520" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="520" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A520" t="s">
         <v>247</v>
       </c>
@@ -19165,7 +19166,7 @@
         <v>3.7881300000000002</v>
       </c>
     </row>
-    <row r="521" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="521" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A521" t="s">
         <v>247</v>
       </c>
@@ -19194,7 +19195,7 @@
         <v>1.4192400000000001</v>
       </c>
     </row>
-    <row r="522" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="522" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A522" t="s">
         <v>247</v>
       </c>
@@ -19223,7 +19224,7 @@
         <v>2.3688899999999999</v>
       </c>
     </row>
-    <row r="523" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="523" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A523" t="s">
         <v>247</v>
       </c>
@@ -19252,7 +19253,7 @@
         <v>2.3688899999999999</v>
       </c>
     </row>
-    <row r="524" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="524" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A524" t="s">
         <v>247</v>
       </c>
@@ -19310,7 +19311,7 @@
         <v>6.9180999999999995E-4</v>
       </c>
     </row>
-    <row r="526" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="526" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A526" t="s">
         <v>247</v>
       </c>
@@ -19368,7 +19369,7 @@
         <v>0.709955</v>
       </c>
     </row>
-    <row r="528" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="528" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A528" t="s">
         <v>247</v>
       </c>
@@ -19426,7 +19427,7 @@
         <v>0.44364700000000001</v>
       </c>
     </row>
-    <row r="530" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="530" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A530" t="s">
         <v>247</v>
       </c>
@@ -19484,7 +19485,7 @@
         <v>0.44284800000000002</v>
       </c>
     </row>
-    <row r="532" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="532" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A532" t="s">
         <v>247</v>
       </c>
@@ -19513,7 +19514,7 @@
         <v>2424.89</v>
       </c>
     </row>
-    <row r="533" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="533" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A533" t="s">
         <v>247</v>
       </c>
@@ -19542,7 +19543,7 @@
         <v>1233.5999999999999</v>
       </c>
     </row>
-    <row r="534" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="534" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A534" t="s">
         <v>247</v>
       </c>
@@ -19571,7 +19572,7 @@
         <v>1191.3</v>
       </c>
     </row>
-    <row r="535" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="535" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A535" t="s">
         <v>247</v>
       </c>
@@ -19600,7 +19601,7 @@
         <v>5720.81</v>
       </c>
     </row>
-    <row r="536" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="536" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A536" t="s">
         <v>247</v>
       </c>
@@ -19629,7 +19630,7 @@
         <v>493.07400000000001</v>
       </c>
     </row>
-    <row r="537" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="537" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A537" t="s">
         <v>247</v>
       </c>
@@ -19687,7 +19688,7 @@
         <v>3.1805199999999999E-2</v>
       </c>
     </row>
-    <row r="539" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="539" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A539" t="s">
         <v>247</v>
       </c>
@@ -19745,7 +19746,7 @@
         <v>1.6153500000000001E-2</v>
       </c>
     </row>
-    <row r="541" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="541" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A541" t="s">
         <v>247</v>
       </c>
@@ -19803,7 +19804,7 @@
         <v>1.5651700000000001E-2</v>
       </c>
     </row>
-    <row r="543" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="543" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A543" t="s">
         <v>247</v>
       </c>
@@ -19861,7 +19862,7 @@
         <v>1.4778700000000001E-2</v>
       </c>
     </row>
-    <row r="545" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="545" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A545" t="s">
         <v>247</v>
       </c>
@@ -19919,7 +19920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="547" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="547" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A547" t="s">
         <v>247</v>
       </c>
@@ -19977,7 +19978,7 @@
         <v>6.9414599999999998E-4</v>
       </c>
     </row>
-    <row r="549" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="549" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A549" t="s">
         <v>247</v>
       </c>
@@ -20035,7 +20036,7 @@
         <v>1.7848699999999999E-4</v>
       </c>
     </row>
-    <row r="551" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="551" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A551" t="s">
         <v>247</v>
       </c>
@@ -20093,7 +20094,7 @@
         <v>1.82626E-4</v>
       </c>
     </row>
-    <row r="553" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="553" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A553" t="s">
         <v>247</v>
       </c>
@@ -20151,7 +20152,7 @@
         <v>7.29968E-4</v>
       </c>
     </row>
-    <row r="555" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="555" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A555" t="s">
         <v>247</v>
       </c>
@@ -20180,7 +20181,7 @@
         <v>3.9970699999999999</v>
       </c>
     </row>
-    <row r="556" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="556" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A556" t="s">
         <v>247</v>
       </c>
@@ -20209,7 +20210,7 @@
         <v>0.59411599999999998</v>
       </c>
     </row>
-    <row r="557" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="557" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A557" t="s">
         <v>247</v>
       </c>
@@ -20267,7 +20268,7 @@
         <v>6.0557299999999997E-5</v>
       </c>
     </row>
-    <row r="559" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="559" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A559" t="s">
         <v>247</v>
       </c>
@@ -20296,7 +20297,7 @@
         <v>0.331592</v>
       </c>
     </row>
-    <row r="560" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="560" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A560" t="s">
         <v>247</v>
       </c>
@@ -20354,7 +20355,7 @@
         <v>0.16761499999999999</v>
       </c>
     </row>
-    <row r="562" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="562" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A562" t="s">
         <v>247</v>
       </c>
@@ -20412,7 +20413,7 @@
         <v>0.61046299999999998</v>
       </c>
     </row>
-    <row r="564" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="564" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A564" t="s">
         <v>247</v>
       </c>
@@ -20441,7 +20442,7 @@
         <v>3342.7</v>
       </c>
     </row>
-    <row r="565" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="565" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A565" t="s">
         <v>247</v>
       </c>
@@ -20470,7 +20471,7 @@
         <v>156.083</v>
       </c>
     </row>
-    <row r="566" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="566" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A566" t="s">
         <v>247</v>
       </c>
@@ -26821,7 +26822,7 @@
         <v>1962.95</v>
       </c>
     </row>
-    <row r="785" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="785" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A785" t="s">
         <v>247</v>
       </c>
@@ -26850,7 +26851,7 @@
         <v>86.926699999999997</v>
       </c>
     </row>
-    <row r="786" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="786" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A786" t="s">
         <v>247</v>
       </c>
@@ -26879,7 +26880,7 @@
         <v>8.7534393809114377</v>
       </c>
     </row>
-    <row r="787" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="787" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A787" t="s">
         <v>247</v>
       </c>
@@ -26912,7 +26913,9 @@
   <autoFilter ref="A1:I787" xr:uid="{8207FD8A-565E-46DA-BF84-876AE3AB2369}">
     <filterColumn colId="5">
       <filters>
-        <filter val="GW"/>
+        <filter val="USD per barrel (2022, MER)"/>
+        <filter val="USD per GJ (2022, MER)"/>
+        <filter val="USD per tonne (2022, MER)"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -30696,7 +30699,7 @@
         <v>449</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" ref="F34:F65" si="1">INDEX(C:C, MATCH(E34,B:B,0))</f>
+        <f t="shared" ref="F34:F51" si="1">INDEX(C:C, MATCH(E34,B:B,0))</f>
         <v>Y</v>
       </c>
     </row>

</xml_diff>